<commit_message>
Corrected "Fats oils and greases" to "Animal Fat" for HEFA
</commit_message>
<xml_diff>
--- a/data/SJV Portfolio - Amplify Bioenergy Buildout 2.1.2024.xlsx
+++ b/data/SJV Portfolio - Amplify Bioenergy Buildout 2.1.2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nidhi/Library/CloudStorage/OneDrive-RANDCorporation/CATF/SJV-/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB4BC34-8A06-E449-B196-6AA1BBD148E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3497E7C-2771-6A4C-842E-3C62580096FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20800" xr2:uid="{3EB5D1B8-C67A-D54A-8FBA-1478F31DBAA7}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="20800" activeTab="2" xr2:uid="{3EB5D1B8-C67A-D54A-8FBA-1478F31DBAA7}"/>
   </bookViews>
   <sheets>
     <sheet name="portfolio_input" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="104">
   <si>
     <t>Solar</t>
   </si>
@@ -430,6 +430,9 @@
   </si>
   <si>
     <t>This portfolio uses half of the available biomass, split out across the different pathways to amplify the bioenergy production. The rest of the portfolio is aligned with the "proportional" effort</t>
+  </si>
+  <si>
+    <t>Animal Fat</t>
   </si>
 </sst>
 </file>
@@ -986,7 +989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA35989-F8F5-C645-8F8C-CB2D79A95BD0}">
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="133" workbookViewId="0">
+    <sheetView topLeftCell="A3" zoomScale="133" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -1809,8 +1812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{225537EC-F8DB-7B4E-B90C-2D6AA935C6A7}">
   <dimension ref="A1:AA20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA9" sqref="AA2:AA9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3780,8 +3783,8 @@
       <c r="A20" t="s">
         <v>52</v>
       </c>
-      <c r="B20" t="s">
-        <v>52</v>
+      <c r="B20" s="22" t="s">
+        <v>103</v>
       </c>
       <c r="C20" t="s">
         <v>74</v>

</xml_diff>